<commit_message>
Add Accuracy Results After Oversampling
</commit_message>
<xml_diff>
--- a/Accuracy Sheet.xlsx
+++ b/Accuracy Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17150"/>
+    <workbookView windowWidth="19200" windowHeight="17600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t>8s Time Window</t>
+  </si>
+  <si>
+    <t>8s Time Window With Oversampling</t>
   </si>
   <si>
     <t>Test Participant</t>
@@ -429,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -450,6 +453,39 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -576,7 +612,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -588,34 +624,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -700,7 +736,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -710,13 +746,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1255,402 +1300,744 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:F24"/>
+  <dimension ref="B1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="6" width="20.4545454545455" customWidth="1"/>
+    <col min="10" max="14" width="20.4545454545455" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.5" spans="2:2">
+    <row r="1" ht="17.5" spans="2:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" ht="15.25"/>
-    <row r="3" ht="20" customHeight="1" spans="2:6">
+    <row r="3" ht="20" customHeight="1" spans="2:14">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" ht="20" customHeight="1" spans="2:6">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="N3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="2:14">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
         <v>0.812206572769953</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>20</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>325</v>
       </c>
-    </row>
-    <row r="5" ht="20" customHeight="1" spans="2:6">
-      <c r="B5" s="3">
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.978292329956584</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.857142857142857</v>
+      </c>
+      <c r="M4" s="3">
+        <v>10</v>
+      </c>
+      <c r="N4" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="2:14">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>0.996153846153846</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>0.825892857142857</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>15</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>350</v>
       </c>
-    </row>
-    <row r="6" ht="20" customHeight="1" spans="2:6">
-      <c r="B6" s="3">
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.85204081632653</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="2:14">
+      <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>0.997439180537772</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>0.89090909090909</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>15</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>250</v>
       </c>
-    </row>
-    <row r="7" ht="20" customHeight="1" spans="2:6">
-      <c r="B7" s="3">
+      <c r="J6" s="2">
+        <v>3</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.908163265306122</v>
+      </c>
+      <c r="M6" s="3">
+        <v>15</v>
+      </c>
+      <c r="N6" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="2:14">
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
         <v>0.796208530805687</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3">
+        <v>200</v>
+      </c>
+      <c r="J7" s="2">
+        <v>4</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.862244897959183</v>
+      </c>
+      <c r="M7" s="3">
+        <v>20</v>
+      </c>
+      <c r="N7" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="2:14">
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.924242424242424</v>
+      </c>
+      <c r="E8" s="3">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3">
+        <v>250</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.997167138810198</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0.982300884955752</v>
+      </c>
+      <c r="M8" s="3">
+        <v>15</v>
+      </c>
+      <c r="N8" s="3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="2:14">
+      <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="F7" s="4">
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.863636363636363</v>
+      </c>
+      <c r="E9" s="3">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3">
+        <v>325</v>
+      </c>
+      <c r="J9" s="2">
+        <v>6</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0.888888888888888</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="2:14">
+      <c r="B10" s="2">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.991217063989962</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.797101449275362</v>
+      </c>
+      <c r="E10" s="3">
+        <v>15</v>
+      </c>
+      <c r="F10" s="3">
+        <v>350</v>
+      </c>
+      <c r="J10" s="2">
+        <v>7</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.997155049786628</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.821705426356589</v>
+      </c>
+      <c r="M10" s="3">
+        <v>15</v>
+      </c>
+      <c r="N10" s="3">
         <v>200</v>
       </c>
     </row>
-    <row r="8" ht="20" customHeight="1" spans="2:6">
-      <c r="B8" s="3">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.924242424242424</v>
-      </c>
-      <c r="E8" s="4">
+    <row r="11" ht="20" customHeight="1" spans="2:14">
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.994993742177722</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.856060606060606</v>
+      </c>
+      <c r="E11" s="3">
+        <v>15</v>
+      </c>
+      <c r="F11" s="3">
+        <v>225</v>
+      </c>
+      <c r="J11" s="2">
+        <v>8</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0.870689655172413</v>
+      </c>
+      <c r="M11" s="3">
+        <v>15</v>
+      </c>
+      <c r="N11" s="3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="2:14">
+      <c r="B12" s="2">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.997448979591836</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.883495145631068</v>
+      </c>
+      <c r="E12" s="3">
+        <v>15</v>
+      </c>
+      <c r="F12" s="3">
+        <v>325</v>
+      </c>
+      <c r="J12" s="2">
+        <v>9</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.901639344262295</v>
+      </c>
+      <c r="M12" s="3">
         <v>20</v>
       </c>
-      <c r="F8" s="4">
+      <c r="N12" s="3">
         <v>250</v>
       </c>
     </row>
-    <row r="9" ht="20" customHeight="1" spans="2:6">
-      <c r="B9" s="3">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.863636363636363</v>
-      </c>
-      <c r="E9" s="4">
+    <row r="13" ht="20" customHeight="1" spans="2:14">
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.852017937219731</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3">
+        <v>250</v>
+      </c>
+      <c r="J13" s="2">
+        <v>10</v>
+      </c>
+      <c r="K13" s="7">
+        <v>1</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0.883495145631068</v>
+      </c>
+      <c r="M13" s="3">
+        <v>15</v>
+      </c>
+      <c r="N13" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1" spans="2:14">
+      <c r="B14" s="2">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.992307692307692</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.897321428571428</v>
+      </c>
+      <c r="E14" s="3">
+        <v>15</v>
+      </c>
+      <c r="F14" s="3">
+        <v>325</v>
+      </c>
+      <c r="J14" s="2">
+        <v>11</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0.924324324324324</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1" spans="2:14">
+      <c r="B15" s="2">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.99359795134443</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.86697247706422</v>
+      </c>
+      <c r="E15" s="3">
+        <v>15</v>
+      </c>
+      <c r="F15" s="3">
+        <v>200</v>
+      </c>
+      <c r="J15" s="2">
+        <v>12</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0.998552821997105</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.915343915343915</v>
+      </c>
+      <c r="M15" s="3">
+        <v>15</v>
+      </c>
+      <c r="N15" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1" spans="2:14">
+      <c r="B16" s="2">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.997435897435897</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.831858407079646</v>
+      </c>
+      <c r="E16" s="3">
+        <v>15</v>
+      </c>
+      <c r="F16" s="3">
+        <v>325</v>
+      </c>
+      <c r="J16" s="2">
+        <v>13</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.851282051282051</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16" s="3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="2:14">
+      <c r="B17" s="2">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.808290155440414</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3">
+        <v>250</v>
+      </c>
+      <c r="J17" s="2">
+        <v>14</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0.998563218390804</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.877300613496932</v>
+      </c>
+      <c r="M17" s="3">
+        <v>15</v>
+      </c>
+      <c r="N17" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="2:14">
+      <c r="B18" s="2">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.84375</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="3">
+        <v>250</v>
+      </c>
+      <c r="J18" s="2">
+        <v>15</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0.897959183673469</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1" spans="2:14">
+      <c r="B19" s="2">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.836283185840707</v>
+      </c>
+      <c r="E19" s="3">
         <v>20</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F19" s="3">
+        <v>225</v>
+      </c>
+      <c r="J19" s="2">
+        <v>16</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="8">
+        <v>0.871287128712871</v>
+      </c>
+      <c r="M19" s="3">
+        <v>20</v>
+      </c>
+      <c r="N19" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" spans="2:14">
+      <c r="B20" s="2">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.844036697247706</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="3">
+        <v>225</v>
+      </c>
+      <c r="J20" s="2">
+        <v>17</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0.997101449275362</v>
+      </c>
+      <c r="L20" s="8">
+        <v>0.854922279792746</v>
+      </c>
+      <c r="M20" s="3">
+        <v>15</v>
+      </c>
+      <c r="N20" s="3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1" spans="2:14">
+      <c r="B21" s="2">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.809734513274336</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3">
+        <v>250</v>
+      </c>
+      <c r="J21" s="2">
+        <v>18</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0.837563451776649</v>
+      </c>
+      <c r="M21" s="3">
+        <v>20</v>
+      </c>
+      <c r="N21" s="3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1" spans="2:14">
+      <c r="B22" s="2">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.997439180537772</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.81081081081081</v>
+      </c>
+      <c r="E22" s="3">
+        <v>15</v>
+      </c>
+      <c r="F22" s="3">
+        <v>300</v>
+      </c>
+      <c r="J22" s="2">
+        <v>19</v>
+      </c>
+      <c r="K22" s="3">
+        <v>1</v>
+      </c>
+      <c r="L22" s="8">
+        <v>0.857843137254901</v>
+      </c>
+      <c r="M22" s="3">
+        <v>20</v>
+      </c>
+      <c r="N22" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1" spans="2:14">
+      <c r="B23" s="2">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.993589743589743</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.814977973568281</v>
+      </c>
+      <c r="E23" s="3">
+        <v>15</v>
+      </c>
+      <c r="F23" s="3">
+        <v>200</v>
+      </c>
+      <c r="J23" s="2">
+        <v>20</v>
+      </c>
+      <c r="K23" s="3">
+        <v>1</v>
+      </c>
+      <c r="L23" s="8">
+        <v>0.82051282051282</v>
+      </c>
+      <c r="M23" s="3">
+        <v>20</v>
+      </c>
+      <c r="N23" s="3">
         <v>325</v>
       </c>
     </row>
-    <row r="10" ht="20" customHeight="1" spans="2:6">
-      <c r="B10" s="3">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.991217063989962</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0.797101449275362</v>
-      </c>
-      <c r="E10" s="4">
-        <v>15</v>
-      </c>
-      <c r="F10" s="4">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" ht="20" customHeight="1" spans="2:6">
-      <c r="B11" s="3">
+    <row r="24" ht="18.25" spans="2:14">
+      <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6">
-        <v>0.994993742177722</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0.856060606060606</v>
-      </c>
-      <c r="E11" s="4">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="12" ht="20" customHeight="1" spans="2:6">
-      <c r="B12" s="3">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.997448979591836</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0.883495145631068</v>
-      </c>
-      <c r="E12" s="4">
-        <v>15</v>
-      </c>
-      <c r="F12" s="4">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="13" ht="20" customHeight="1" spans="2:6">
-      <c r="B13" s="3">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.852017937219731</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="14" ht="20" customHeight="1" spans="2:6">
-      <c r="B14" s="3">
-        <v>11</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.992307692307692</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0.897321428571428</v>
-      </c>
-      <c r="E14" s="4">
-        <v>15</v>
-      </c>
-      <c r="F14" s="4">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="15" ht="20" customHeight="1" spans="2:6">
-      <c r="B15" s="3">
-        <v>12</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0.99359795134443</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0.86697247706422</v>
-      </c>
-      <c r="E15" s="4">
-        <v>15</v>
-      </c>
-      <c r="F15" s="4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" ht="20" customHeight="1" spans="2:6">
-      <c r="B16" s="3">
-        <v>13</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0.997435897435897</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0.831858407079646</v>
-      </c>
-      <c r="E16" s="4">
-        <v>15</v>
-      </c>
-      <c r="F16" s="4">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="17" ht="20" customHeight="1" spans="2:6">
-      <c r="B17" s="3">
-        <v>14</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0.808290155440414</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" ht="20" customHeight="1" spans="2:6">
-      <c r="B18" s="3">
-        <v>15</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0.84375</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" ht="20" customHeight="1" spans="2:6">
-      <c r="B19" s="3">
-        <v>16</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0.836283185840707</v>
-      </c>
-      <c r="E19" s="4">
-        <v>20</v>
-      </c>
-      <c r="F19" s="4">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" ht="20" customHeight="1" spans="2:6">
-      <c r="B20" s="3">
-        <v>17</v>
-      </c>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0.844036697247706</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="4">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" ht="20" customHeight="1" spans="2:6">
-      <c r="B21" s="3">
-        <v>18</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0.809734513274336</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="22" ht="20" customHeight="1" spans="2:6">
-      <c r="B22" s="3">
-        <v>19</v>
-      </c>
-      <c r="C22" s="6">
-        <v>0.997439180537772</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0.81081081081081</v>
-      </c>
-      <c r="E22" s="4">
-        <v>15</v>
-      </c>
-      <c r="F22" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="23" ht="20" customHeight="1" spans="2:6">
-      <c r="B23" s="3">
-        <v>20</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0.993589743589743</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0.814977973568281</v>
-      </c>
-      <c r="E23" s="4">
-        <v>15</v>
-      </c>
-      <c r="F23" s="4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" ht="18.25" spans="2:6">
-      <c r="B24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <f>SUM(C4:C23)/COUNT(C4:C23)</f>
         <v>0.997581163883334</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="3">
         <f>SUM(D4:D23)/COUNT(D4:D23)</f>
         <v>0.843290331329534</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="3">
         <f>SUM(E4:E23)/COUNT(E4:E23)</f>
         <v>16.4285714285714</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="3">
         <f>SUM(F4:F23)/COUNT(F4:F23)</f>
         <v>270</v>
       </c>
+      <c r="J24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" ref="K24:N24" si="0">SUM(K4:K23)/COUNT(K4:K23)</f>
+        <v>0.998341600410834</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="0"/>
+        <v>0.876832504408619</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="0"/>
+        <v>16.6666666666667</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
accuracy sheet and featuires score saved for 8s window
</commit_message>
<xml_diff>
--- a/Accuracy Sheet.xlsx
+++ b/Accuracy Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravik\Desktop\project_work_stairs_lift_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51485E9-7F94-4EFD-9B93-1A377F486FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42ACF7F-4A2B-4564-9F8B-7178BB0E393C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="8s window" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Test Participant</t>
   </si>
@@ -724,7 +724,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -834,16 +834,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>0.86224489795918302</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+        <v>0.82383419689119097</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.82383419689119097</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.81102705277875597</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.82562283797952796</v>
+      </c>
       <c r="F5" s="3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>9</v>
@@ -854,16 +860,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="6">
-        <v>0.98230088495575196</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+        <v>0.95535714285714202</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.95535714285714202</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.94081310960702003</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.95542722583538897</v>
+      </c>
       <c r="F6" s="3">
         <v>15</v>
       </c>
       <c r="G6" s="3">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>10</v>
@@ -874,16 +886,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <v>0.88888888888888795</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="3" t="s">
-        <v>4</v>
+        <v>0.87309644670050701</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.87309644670050701</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.85661779081133904</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.87367043741695705</v>
+      </c>
+      <c r="F7" s="3">
+        <v>20</v>
       </c>
       <c r="G7" s="3">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>11</v>
@@ -894,16 +912,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="6">
-        <v>0.82170542635658905</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+        <v>0.8125</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.8125</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.79407366209368402</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.81528400576257498</v>
+      </c>
       <c r="F8" s="3">
         <v>15</v>
       </c>
       <c r="G8" s="3">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>12</v>
@@ -915,16 +939,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="6">
-        <v>0.87068965517241304</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+        <v>0.88695652173912998</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.88695652173912998</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.80882722857529799</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.88328752556443602</v>
+      </c>
       <c r="F9" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G9" s="3">
-        <v>275</v>
+        <v>200</v>
       </c>
       <c r="J9" s="10"/>
     </row>
@@ -933,16 +963,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="6">
-        <v>0.90163934426229497</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="3">
-        <v>20</v>
+        <v>0.9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.87087351556189496</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.89705814960142005</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="G10" s="3">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="J10" s="10"/>
     </row>
@@ -951,16 +987,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="7">
-        <v>0.88349514563106801</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+        <v>0.90640394088669896</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.90640394088669896</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.85485214950697197</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.90302617691227505</v>
+      </c>
       <c r="F11" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G11" s="3">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="J11" s="10"/>
     </row>
@@ -969,16 +1011,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="6">
-        <v>0.92432432432432399</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.90966315148035504</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.92284961247957398</v>
+      </c>
       <c r="F12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="3">
-        <v>275</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="20" customHeight="1" thickBot="1">
@@ -986,16 +1034,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="6">
-        <v>0.91534391534391502</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+        <v>0.89839572192513295</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.89839572192513295</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.89719412137376497</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.89961161250624599</v>
+      </c>
       <c r="F13" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G13" s="3">
-        <v>225</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="20" customHeight="1" thickBot="1">
@@ -1003,16 +1057,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="6">
-        <v>0.85128205128205103</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="3" t="s">
-        <v>4</v>
+        <v>0.865979381443299</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.865979381443299</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.86880711880711803</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.862081541978449</v>
+      </c>
+      <c r="F14" s="3">
+        <v>20</v>
       </c>
       <c r="G14" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="20" customHeight="1" thickBot="1">
@@ -1020,16 +1080,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="6">
-        <v>0.877300613496932</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="3">
-        <v>15</v>
+        <v>0.88888888888888795</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.88888888888888795</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.87948075893653699</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.88848062162362595</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="G15" s="3">
-        <v>200</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="20" customHeight="1" thickBot="1">
@@ -1037,16 +1103,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="6">
-        <v>0.89795918367346905</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="3" t="s">
-        <v>4</v>
+        <v>0.86528497409326399</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.86528497409326399</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.87236581048762496</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.86932347679020905</v>
+      </c>
+      <c r="F16" s="3">
+        <v>15</v>
       </c>
       <c r="G16" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" thickBot="1">
@@ -1054,13 +1126,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="6">
-        <v>0.87128712871287095</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="3">
-        <v>20</v>
+        <v>0.87562189054726303</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.87562189054726303</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.888942569868442</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.87479546587087298</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="G17" s="3">
         <v>300</v>
@@ -1071,16 +1149,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="6">
-        <v>0.85492227979274604</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3">
-        <v>15</v>
+        <v>0.859375</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.859375</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.818063493456062</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.85897172992368398</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="G18" s="3">
-        <v>225</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1" thickBot="1">
@@ -1088,16 +1172,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="6">
-        <v>0.83756345177664904</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+        <v>0.87755102040816302</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0.87755102040816302</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.88119665527245095</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.878369238553381</v>
+      </c>
       <c r="F19" s="3">
         <v>20</v>
       </c>
       <c r="G19" s="3">
-        <v>350</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1" thickBot="1">
@@ -1105,16 +1195,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="6">
-        <v>0.85784313725490102</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+        <v>0.86274509803921495</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.86274509803921495</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.79089720218752402</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.86298497695556498</v>
+      </c>
       <c r="F20" s="3">
         <v>20</v>
       </c>
       <c r="G20" s="3">
-        <v>250</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1" thickBot="1">
@@ -1145,19 +1241,28 @@
         <v>5</v>
       </c>
       <c r="B22" s="8">
-        <f t="shared" ref="B22:G22" si="0">SUM(B2:B21)/COUNT(B2:B21)</f>
-        <v>0.8772870352347123</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+        <f>SUM(B2:B21)/COUNT(B2:B21)</f>
+        <v>0.87610087616535082</v>
+      </c>
+      <c r="C22" s="8">
+        <f>SUM(C2:C21)/COUNT(C2:C21)</f>
+        <v>0.87610087616535082</v>
+      </c>
+      <c r="D22" s="8">
+        <f>SUM(D2:D21)/COUNT(D2:D21)</f>
+        <v>0.85627449729035876</v>
+      </c>
+      <c r="E22" s="8">
+        <f>SUM(E2:E21)/COUNT(E2:E21)</f>
+        <v>0.87566552064708714</v>
+      </c>
       <c r="F22" s="3">
-        <f t="shared" si="0"/>
-        <v>17.307692307692307</v>
+        <f t="shared" ref="B22:G22" si="0">SUM(F2:F21)/COUNT(F2:F21)</f>
+        <v>18.333333333333332</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="0"/>
-        <v>263.75</v>
+        <v>258.75</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1"/>

</xml_diff>

<commit_message>
accuracy sheet updated for 4s window
</commit_message>
<xml_diff>
--- a/Accuracy Sheet.xlsx
+++ b/Accuracy Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravik\Desktop\project_work_stairs_lift_detection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrish\Downloads\project_work_stairs_lift_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42ACF7F-4A2B-4564-9F8B-7178BB0E393C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4630A2C9-9A5C-4F1B-AD3F-05BC3C2DA037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="8s window" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
   <si>
     <t>Test Participant</t>
   </si>
@@ -131,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -187,13 +187,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -232,6 +247,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1257,7 +1293,7 @@
         <v>0.87566552064708714</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" ref="B22:G22" si="0">SUM(F2:F21)/COUNT(F2:F21)</f>
+        <f t="shared" ref="F22:G22" si="0">SUM(F2:F21)/COUNT(F2:F21)</f>
         <v>18.333333333333332</v>
       </c>
       <c r="G22" s="3">
@@ -1274,12 +1310,537 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967678E6-06EA-415A-8B69-E208F497A1B1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17.5">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17.5">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18">
+        <v>0.77192982456140302</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0.77192982456140302</v>
+      </c>
+      <c r="D2" s="15">
+        <v>0.72330359066299199</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0.77298234493960905</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="15">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.5">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0.81294964028776895</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.81294964028776895</v>
+      </c>
+      <c r="D3" s="15">
+        <v>0.75160817276508096</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0.80443910660606899</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="15">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.5">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.81204819277108398</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0.81204819277108398</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0.75742893041252801</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.809110965493545</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17.5">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.77443609022556303</v>
+      </c>
+      <c r="C5" s="15">
+        <v>0.77443609022556303</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.72818488970796202</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.77620630988546602</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="15">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.5">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.77777777777777701</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0.77777777777777701</v>
+      </c>
+      <c r="D6" s="15">
+        <v>0.73177358157387795</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.78176514103276395</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.5">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.794258373205741</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0.794258373205741</v>
+      </c>
+      <c r="D7" s="15">
+        <v>0.76119929296278399</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.79417359708031698</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17.5">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0.747169811320754</v>
+      </c>
+      <c r="C8" s="15">
+        <v>0.747169811320754</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.71975106447734505</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.75843660172189598</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17.5">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18">
+        <v>0.77822580645161199</v>
+      </c>
+      <c r="C9" s="15">
+        <v>0.77822580645161199</v>
+      </c>
+      <c r="D9" s="15">
+        <v>0.74715513989900795</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0.77296835719749701</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="15">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17.5">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18">
+        <v>0.84656084656084596</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0.84656084656084596</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.79581099940442801</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0.84168988186539695</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.5">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0.83649289099526003</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.83649289099526003</v>
+      </c>
+      <c r="D11" s="15">
+        <v>0.70205753846637398</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.83047332397935003</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="15">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.5">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="18">
+        <v>0.87376237623762298</v>
+      </c>
+      <c r="C12" s="15">
+        <v>0.87376237623762298</v>
+      </c>
+      <c r="D12" s="15">
+        <v>0.86747083775185496</v>
+      </c>
+      <c r="E12" s="15">
+        <v>0.87359602542968995</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="15">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17.5">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0.79706601466992599</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0.79706601466992599</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.77693946887299703</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.79735035762501405</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="15">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17.5">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.79383886255924097</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0.79383886255924097</v>
+      </c>
+      <c r="D14" s="15">
+        <v>0.73491044257197702</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.78677565635058699</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17.5">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
+      <c r="B15" s="18">
+        <v>0.800561797752809</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0.800561797752809</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0.72312521329948198</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.79646917202705003</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="15">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.5">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0.82608695652173902</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.82608695652173902</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0.82284069205617105</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.82690336988109903</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="15">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.5">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" s="18">
+        <v>0.81411764705882295</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0.81411764705882295</v>
+      </c>
+      <c r="D17" s="15">
+        <v>0.79300392843871104</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0.811098801170412</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17.5">
+      <c r="A18" s="13">
+        <v>17</v>
+      </c>
+      <c r="B18" s="18">
+        <v>0.79411764705882304</v>
+      </c>
+      <c r="C18" s="15">
+        <v>0.79411764705882304</v>
+      </c>
+      <c r="D18" s="15">
+        <v>0.74361322141208297</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0.79174884813069801</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="15">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17.5">
+      <c r="A19" s="13">
+        <v>18</v>
+      </c>
+      <c r="B19" s="18">
+        <v>0.77163461538461497</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0.77163461538461497</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0.770138228782144</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0.77081693658085604</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="15">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17.5">
+      <c r="A20" s="13">
+        <v>19</v>
+      </c>
+      <c r="B20" s="18">
+        <v>0.82783018867924496</v>
+      </c>
+      <c r="C20" s="15">
+        <v>0.82783018867924496</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0.77764420401075696</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0.82729811997018499</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="15">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17.5">
+      <c r="A21" s="13">
+        <v>20</v>
+      </c>
+      <c r="B21" s="18">
+        <v>0.76626506024096297</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0.76626506024096297</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0.73164926382361695</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0.76056459524476805</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17.5">
+      <c r="A22" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="19">
+        <f>AVERAGE(B2:B21)</f>
+        <v>0.80085652101608074</v>
+      </c>
+      <c r="C22" s="17">
+        <f>SUM(C2:C21)/COUNT(C2:C21)</f>
+        <v>0.80085652101608074</v>
+      </c>
+      <c r="D22" s="17">
+        <f>SUM(D2:D21)/COUNT(D2:D21)</f>
+        <v>0.7579804350676087</v>
+      </c>
+      <c r="E22" s="17">
+        <f>SUM(E2:E21)/COUNT(E2:E21)</f>
+        <v>0.79924337561061343</v>
+      </c>
+      <c r="F22" s="15" t="e">
+        <f t="shared" ref="F22:G22" si="0">SUM(F2:F21)/COUNT(F2:F21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="15">
+        <f t="shared" si="0"/>
+        <v>277.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
confusion matrices for 8s window
</commit_message>
<xml_diff>
--- a/Accuracy Sheet.xlsx
+++ b/Accuracy Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravik\Desktop\project_work_stairs_lift_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42ACF7F-4A2B-4564-9F8B-7178BB0E393C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002F2B05-8517-4854-8435-5BF59CA7E51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Test Participant</t>
   </si>
@@ -59,18 +59,6 @@
   </si>
   <si>
     <t>F1Score(Weighted)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.8404255319148937</t>
-  </si>
-  <si>
-    <t>F1 Score micro: 0.8404255319148937</t>
-  </si>
-  <si>
-    <t>F1 Score macro: 0.8314285714285713</t>
-  </si>
-  <si>
-    <t>F1 Score weighted: 0.8419452887537994</t>
   </si>
 </sst>
 </file>
@@ -723,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -851,9 +839,7 @@
       <c r="G5" s="3">
         <v>275</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:13" ht="20" customHeight="1" thickBot="1">
       <c r="A6" s="2">
@@ -877,9 +863,7 @@
       <c r="G6" s="3">
         <v>250</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="20" customHeight="1" thickBot="1">
       <c r="A7" s="2">
@@ -903,9 +887,7 @@
       <c r="G7" s="3">
         <v>200</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:13" ht="20" customHeight="1" thickBot="1">
       <c r="A8" s="2">
@@ -929,9 +911,7 @@
       <c r="G8" s="3">
         <v>225</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="I8" s="10"/>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:13" ht="20" customHeight="1" thickBot="1">
@@ -1257,7 +1237,7 @@
         <v>0.87566552064708714</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" ref="B22:G22" si="0">SUM(F2:F21)/COUNT(F2:F21)</f>
+        <f t="shared" ref="F22:G22" si="0">SUM(F2:F21)/COUNT(F2:F21)</f>
         <v>18.333333333333332</v>
       </c>
       <c r="G22" s="3">

</xml_diff>